<commit_message>
laboriously fixing the 2000's data pull error calculations
</commit_message>
<xml_diff>
--- a/inputs/2000_census/Census2000SF3_designfac.xlsx
+++ b/inputs/2000_census/Census2000SF3_designfac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaleighTomlin\Desktop\Working Directory\Who-Lives\inputs\2000_census\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE42AF6-0217-4D72-AE59-4607006E8E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1C5D2C-40D0-4807-8B47-B6FE7273E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="2736" windowWidth="17316" windowHeight="14316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>table_name</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>H098</t>
+  </si>
+  <si>
+    <t>P148</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,12 +642,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
@@ -654,26 +668,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D504898F6C39A345BE7DC6B777612B12" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c903bc8010700ac468ab3bd9da055d38">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07a26812-85d3-4425-992a-629e808a49a8" xmlns:ns3="26ce723e-735e-4eb2-8b68-455e42ea4533" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0360ef8260ba8797d0d24b6430bbf7d" ns2:_="" ns3:_="">
     <xsd:import namespace="07a26812-85d3-4425-992a-629e808a49a8"/>
@@ -928,26 +922,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54415AF1-A5BB-449B-9B8C-9787C326D52E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D841BA51-0421-4F4F-970C-7C7E6CAB9970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
-    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFA27836-89D4-4212-A427-52AEA29C0E56}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -964,4 +959,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D841BA51-0421-4F4F-970C-7C7E6CAB9970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
+    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54415AF1-A5BB-449B-9B8C-9787C326D52E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixing manual 2000s stuff still. sad face
</commit_message>
<xml_diff>
--- a/inputs/2000_census/Census2000SF3_designfac.xlsx
+++ b/inputs/2000_census/Census2000SF3_designfac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaleighTomlin\Desktop\Working Directory\Who-Lives\inputs\2000_census\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1C5D2C-40D0-4807-8B47-B6FE7273E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3094FA6-0ABD-4BB6-8760-316AB1712A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="0" windowWidth="11460" windowHeight="14410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>table_name</t>
   </si>
@@ -93,13 +93,16 @@
   </si>
   <si>
     <t>P148</t>
+  </si>
+  <si>
+    <t>H004</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,18 +467,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -497,7 +500,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -508,7 +511,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -519,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -530,7 +533,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -541,7 +544,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -552,7 +555,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -563,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -574,7 +577,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -585,7 +588,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -596,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -607,7 +610,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -618,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -629,7 +632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -640,7 +643,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -651,14 +654,25 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>1</v>
       </c>
     </row>
@@ -668,6 +682,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D504898F6C39A345BE7DC6B777612B12" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c903bc8010700ac468ab3bd9da055d38">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07a26812-85d3-4425-992a-629e808a49a8" xmlns:ns3="26ce723e-735e-4eb2-8b68-455e42ea4533" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0360ef8260ba8797d0d24b6430bbf7d" ns2:_="" ns3:_="">
     <xsd:import namespace="07a26812-85d3-4425-992a-629e808a49a8"/>
@@ -922,27 +956,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="07a26812-85d3-4425-992a-629e808a49a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="26ce723e-735e-4eb2-8b68-455e42ea4533" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54415AF1-A5BB-449B-9B8C-9787C326D52E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D841BA51-0421-4F4F-970C-7C7E6CAB9970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
+    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFA27836-89D4-4212-A427-52AEA29C0E56}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -959,23 +992,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D841BA51-0421-4F4F-970C-7C7E6CAB9970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="07a26812-85d3-4425-992a-629e808a49a8"/>
-    <ds:schemaRef ds:uri="26ce723e-735e-4eb2-8b68-455e42ea4533"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54415AF1-A5BB-449B-9B8C-9787C326D52E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>